<commit_message>
Platform to Rosinca mortgages.
</commit_message>
<xml_diff>
--- a/data/property/checked/NOV2025_codedAndCategorised.xlsx
+++ b/data/property/checked/NOV2025_codedAndCategorised.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\My Drive\NAS\My Documents\Business\Property\Statements\working\python\data\property\checked\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Mat\property\data\property\checked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E9DD0757-96FA-4D62-B14C-AD4A28D0B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E84468F3-04B0-47D0-A450-DA54FCAE8EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09F7DB9E-57D0-4BEE-A79F-4FF06485563A}"/>
+    <workbookView xWindow="30" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{09F7DB9E-57D0-4BEE-A79F-4FF06485563A}"/>
   </bookViews>
   <sheets>
     <sheet name="NOV2025_codedAndCategorised" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="356">
   <si>
     <t>Date</t>
   </si>
@@ -1076,13 +1076,28 @@
   </si>
   <si>
     <t>RSA</t>
+  </si>
+  <si>
+    <t>F5 8</t>
+  </si>
+  <si>
+    <t>F5 4</t>
+  </si>
+  <si>
+    <t>F5 6</t>
+  </si>
+  <si>
+    <t>F3 16</t>
+  </si>
+  <si>
+    <t>F61618ALH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1218,7 +1233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1416,6 +1431,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1577,12 +1598,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1630,6 +1653,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1958,27 +1986,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B6550E-C6E8-4640-92B4-9AD60B0000E3}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" customWidth="1"/>
-    <col min="9" max="9" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45962</v>
       </c>
@@ -2027,7 +2054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45962</v>
       </c>
@@ -2047,7 +2074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45962</v>
       </c>
@@ -2067,7 +2094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45962</v>
       </c>
@@ -2090,7 +2117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45962</v>
       </c>
@@ -2113,7 +2140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45962</v>
       </c>
@@ -2136,7 +2163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45962</v>
       </c>
@@ -2159,7 +2186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45962</v>
       </c>
@@ -2179,7 +2206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45962</v>
       </c>
@@ -2202,7 +2229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45962</v>
       </c>
@@ -2225,7 +2252,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45963</v>
       </c>
@@ -2248,7 +2275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45963</v>
       </c>
@@ -2271,7 +2298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45964</v>
       </c>
@@ -2294,7 +2321,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45964</v>
       </c>
@@ -2317,7 +2344,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45964</v>
       </c>
@@ -2340,7 +2367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45964</v>
       </c>
@@ -2363,7 +2390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45964</v>
       </c>
@@ -2386,7 +2413,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45964</v>
       </c>
@@ -2409,7 +2436,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45964</v>
       </c>
@@ -2432,7 +2459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45964</v>
       </c>
@@ -2448,11 +2475,14 @@
       <c r="E21" t="s">
         <v>51</v>
       </c>
+      <c r="F21" s="6" t="s">
+        <v>261</v>
+      </c>
       <c r="G21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45964</v>
       </c>
@@ -2475,7 +2505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45964</v>
       </c>
@@ -2491,11 +2521,17 @@
       <c r="E23" t="s">
         <v>53</v>
       </c>
+      <c r="F23" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="G23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="H23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45964</v>
       </c>
@@ -2511,11 +2547,14 @@
       <c r="E24" t="s">
         <v>54</v>
       </c>
+      <c r="F24" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45964</v>
       </c>
@@ -2538,7 +2577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45964</v>
       </c>
@@ -2561,7 +2600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45964</v>
       </c>
@@ -2584,7 +2623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45964</v>
       </c>
@@ -2600,11 +2639,17 @@
       <c r="E28" t="s">
         <v>61</v>
       </c>
+      <c r="F28" s="2" t="s">
+        <v>355</v>
+      </c>
       <c r="G28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45964</v>
       </c>
@@ -2627,7 +2672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45964</v>
       </c>
@@ -2647,7 +2692,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45964</v>
       </c>
@@ -2670,7 +2715,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45964</v>
       </c>
@@ -2693,7 +2738,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45964</v>
       </c>
@@ -2714,7 +2759,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45964</v>
       </c>
@@ -2735,7 +2780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45964</v>
       </c>
@@ -2758,7 +2803,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45964</v>
       </c>
@@ -2778,7 +2823,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45964</v>
       </c>
@@ -2801,7 +2846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45964</v>
       </c>
@@ -2824,7 +2869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45964</v>
       </c>
@@ -2847,7 +2892,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45964</v>
       </c>
@@ -2870,7 +2915,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45964</v>
       </c>
@@ -2893,7 +2938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45964</v>
       </c>
@@ -2916,7 +2961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45964</v>
       </c>
@@ -2936,7 +2981,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45964</v>
       </c>
@@ -2956,7 +3001,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45964</v>
       </c>
@@ -2979,7 +3024,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45964</v>
       </c>
@@ -3002,7 +3047,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45964</v>
       </c>
@@ -3025,7 +3070,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45964</v>
       </c>
@@ -3045,7 +3090,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45964</v>
       </c>
@@ -3065,7 +3110,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45964</v>
       </c>
@@ -3085,7 +3130,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45964</v>
       </c>
@@ -3108,7 +3153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45964</v>
       </c>
@@ -3131,7 +3176,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45964</v>
       </c>
@@ -3151,7 +3196,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45964</v>
       </c>
@@ -3171,7 +3216,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45964</v>
       </c>
@@ -3191,7 +3236,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45964</v>
       </c>
@@ -3211,7 +3256,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45964</v>
       </c>
@@ -3231,7 +3276,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45964</v>
       </c>
@@ -3254,7 +3299,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45964</v>
       </c>
@@ -3274,7 +3319,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45965</v>
       </c>
@@ -3297,7 +3342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45965</v>
       </c>
@@ -3320,7 +3365,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45965</v>
       </c>
@@ -3340,7 +3385,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45965</v>
       </c>
@@ -3363,7 +3408,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45965</v>
       </c>
@@ -3383,7 +3428,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45965</v>
       </c>
@@ -3403,7 +3448,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45965</v>
       </c>
@@ -3426,7 +3471,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45965</v>
       </c>
@@ -3449,7 +3494,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45965</v>
       </c>
@@ -3472,7 +3517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45965</v>
       </c>
@@ -3495,7 +3540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45966</v>
       </c>
@@ -3515,7 +3560,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45966</v>
       </c>
@@ -3538,7 +3583,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45966</v>
       </c>
@@ -3561,7 +3606,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45966</v>
       </c>
@@ -3584,7 +3629,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45966</v>
       </c>
@@ -3607,7 +3652,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45966</v>
       </c>
@@ -3630,7 +3675,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45966</v>
       </c>
@@ -3653,7 +3698,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45967</v>
       </c>
@@ -3676,7 +3721,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45967</v>
       </c>
@@ -3696,7 +3741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45967</v>
       </c>
@@ -3719,7 +3764,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45967</v>
       </c>
@@ -3742,7 +3787,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45967</v>
       </c>
@@ -3765,7 +3810,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45967</v>
       </c>
@@ -3788,7 +3833,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45967</v>
       </c>
@@ -3811,7 +3856,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45967</v>
       </c>
@@ -3834,7 +3879,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45967</v>
       </c>
@@ -3857,7 +3902,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45967</v>
       </c>
@@ -3880,7 +3925,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45967</v>
       </c>
@@ -3900,7 +3945,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45968</v>
       </c>
@@ -3923,7 +3968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45968</v>
       </c>
@@ -3946,7 +3991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45968</v>
       </c>
@@ -3966,7 +4011,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45968</v>
       </c>
@@ -3989,7 +4034,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45968</v>
       </c>
@@ -4012,7 +4057,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45968</v>
       </c>
@@ -4035,7 +4080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45968</v>
       </c>
@@ -4058,7 +4103,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45968</v>
       </c>
@@ -4081,7 +4126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45968</v>
       </c>
@@ -4104,7 +4149,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45968</v>
       </c>
@@ -4124,7 +4169,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45968</v>
       </c>
@@ -4147,7 +4192,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45968</v>
       </c>
@@ -4170,7 +4215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45969</v>
       </c>
@@ -4193,7 +4238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45969</v>
       </c>
@@ -4216,7 +4261,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45970</v>
       </c>
@@ -4239,7 +4284,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>45970</v>
       </c>
@@ -4262,7 +4307,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45970</v>
       </c>
@@ -4283,7 +4328,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45970</v>
       </c>
@@ -4306,7 +4351,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>45971</v>
       </c>
@@ -4329,7 +4374,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>45971</v>
       </c>
@@ -4352,7 +4397,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>45971</v>
       </c>
@@ -4375,7 +4420,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45971</v>
       </c>
@@ -4398,7 +4443,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>45971</v>
       </c>
@@ -4421,7 +4466,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>45971</v>
       </c>
@@ -4444,7 +4489,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>45971</v>
       </c>
@@ -4467,7 +4512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>45971</v>
       </c>
@@ -4490,7 +4535,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>45971</v>
       </c>
@@ -4513,7 +4558,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>45971</v>
       </c>
@@ -4536,7 +4581,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>45971</v>
       </c>
@@ -4559,7 +4604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45971</v>
       </c>
@@ -4582,7 +4627,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45971</v>
       </c>
@@ -4605,7 +4650,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>45971</v>
       </c>
@@ -4628,7 +4673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>45972</v>
       </c>
@@ -4651,7 +4696,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>45972</v>
       </c>
@@ -4674,7 +4719,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>45972</v>
       </c>
@@ -4695,7 +4740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>45972</v>
       </c>
@@ -4718,7 +4763,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>45972</v>
       </c>
@@ -4741,7 +4786,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>45972</v>
       </c>
@@ -4764,7 +4809,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>45972</v>
       </c>
@@ -4787,7 +4832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>45972</v>
       </c>
@@ -4810,7 +4855,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>45972</v>
       </c>
@@ -4830,7 +4875,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>45972</v>
       </c>
@@ -4853,7 +4898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>45972</v>
       </c>
@@ -4876,7 +4921,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>45972</v>
       </c>
@@ -4899,7 +4944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>45973</v>
       </c>
@@ -4919,7 +4964,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>45973</v>
       </c>
@@ -4942,7 +4987,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>45973</v>
       </c>
@@ -4965,7 +5010,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>45973</v>
       </c>
@@ -4988,7 +5033,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>45973</v>
       </c>
@@ -5008,7 +5053,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>45973</v>
       </c>
@@ -5031,7 +5076,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>45973</v>
       </c>
@@ -5054,7 +5099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>45973</v>
       </c>
@@ -5077,7 +5122,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>45973</v>
       </c>
@@ -5100,7 +5145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>45974</v>
       </c>
@@ -5123,7 +5168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>45974</v>
       </c>
@@ -5146,7 +5191,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>45974</v>
       </c>
@@ -5169,7 +5214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>45974</v>
       </c>
@@ -5192,7 +5237,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>45974</v>
       </c>
@@ -5215,7 +5260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>45974</v>
       </c>
@@ -5238,7 +5283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>45974</v>
       </c>
@@ -5261,7 +5306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>45974</v>
       </c>
@@ -5284,7 +5329,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>45974</v>
       </c>
@@ -5305,7 +5350,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>45974</v>
       </c>
@@ -5328,7 +5373,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>45975</v>
       </c>
@@ -5348,7 +5393,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>45975</v>
       </c>
@@ -5371,7 +5416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>45975</v>
       </c>
@@ -5394,7 +5439,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>45975</v>
       </c>
@@ -5417,7 +5462,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>45975</v>
       </c>
@@ -5440,7 +5485,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>45975</v>
       </c>
@@ -5463,7 +5508,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>45975</v>
       </c>
@@ -5486,7 +5531,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>45975</v>
       </c>
@@ -5509,7 +5554,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>45976</v>
       </c>
@@ -5532,7 +5577,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>45976</v>
       </c>
@@ -5555,7 +5600,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>45976</v>
       </c>
@@ -5578,7 +5623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>45977</v>
       </c>
@@ -5601,7 +5646,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>45977</v>
       </c>
@@ -5624,7 +5669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>45977</v>
       </c>
@@ -5647,7 +5692,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>45977</v>
       </c>
@@ -5670,7 +5715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>45977</v>
       </c>
@@ -5693,7 +5738,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>45977</v>
       </c>
@@ -5716,7 +5761,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>45978</v>
       </c>
@@ -5739,7 +5784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>45978</v>
       </c>
@@ -5762,7 +5807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>45978</v>
       </c>
@@ -5785,7 +5830,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>45978</v>
       </c>
@@ -5808,7 +5853,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>45978</v>
       </c>
@@ -5828,7 +5873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>45978</v>
       </c>
@@ -5851,7 +5896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>45978</v>
       </c>
@@ -5874,7 +5919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>45978</v>
       </c>
@@ -5894,7 +5939,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>45978</v>
       </c>
@@ -5917,7 +5962,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>45978</v>
       </c>
@@ -5940,7 +5985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>45978</v>
       </c>
@@ -5963,7 +6008,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>45978</v>
       </c>
@@ -5986,7 +6031,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>45978</v>
       </c>
@@ -6009,7 +6054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>45978</v>
       </c>
@@ -6032,7 +6077,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>45978</v>
       </c>
@@ -6055,7 +6100,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>45978</v>
       </c>
@@ -6071,11 +6116,14 @@
       <c r="E183" t="s">
         <v>247</v>
       </c>
+      <c r="F183" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="G183" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>45978</v>
       </c>
@@ -6091,11 +6139,17 @@
       <c r="E184" t="s">
         <v>248</v>
       </c>
+      <c r="F184" s="2" t="s">
+        <v>347</v>
+      </c>
       <c r="G184" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" hidden="1">
+      <c r="H184" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>45978</v>
       </c>
@@ -6115,7 +6169,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>45978</v>
       </c>
@@ -6138,7 +6192,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>45978</v>
       </c>
@@ -6161,7 +6215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>45978</v>
       </c>
@@ -6184,7 +6238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>45978</v>
       </c>
@@ -6200,11 +6254,18 @@
       <c r="E189" t="s">
         <v>252</v>
       </c>
+      <c r="F189" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="G189" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" hidden="1">
+      <c r="H189" t="s">
+        <v>351</v>
+      </c>
+      <c r="I189" s="5"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>45978</v>
       </c>
@@ -6227,7 +6288,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>45979</v>
       </c>
@@ -6248,7 +6309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>45979</v>
       </c>
@@ -6271,7 +6332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>45979</v>
       </c>
@@ -6291,7 +6352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>45979</v>
       </c>
@@ -6314,7 +6375,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>45979</v>
       </c>
@@ -6337,7 +6398,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>45979</v>
       </c>
@@ -6358,7 +6419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>45979</v>
       </c>
@@ -6379,7 +6440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>45979</v>
       </c>
@@ -6402,7 +6463,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>45979</v>
       </c>
@@ -6425,7 +6486,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>45979</v>
       </c>
@@ -6448,7 +6509,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>45979</v>
       </c>
@@ -6471,7 +6532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>45980</v>
       </c>
@@ -6491,7 +6552,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>45980</v>
       </c>
@@ -6514,7 +6575,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>45980</v>
       </c>
@@ -6537,7 +6598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>45980</v>
       </c>
@@ -6560,7 +6621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>45980</v>
       </c>
@@ -6583,7 +6644,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>45981</v>
       </c>
@@ -6606,7 +6667,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>45981</v>
       </c>
@@ -6629,7 +6690,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="209" spans="1:9" hidden="1">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>45981</v>
       </c>
@@ -6652,7 +6713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>45981</v>
       </c>
@@ -6672,7 +6733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>45981</v>
       </c>
@@ -6695,7 +6756,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>45981</v>
       </c>
@@ -6718,7 +6779,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>45981</v>
       </c>
@@ -6741,7 +6802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="214" spans="1:9" hidden="1">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>45981</v>
       </c>
@@ -6761,7 +6822,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>45981</v>
       </c>
@@ -6784,7 +6845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:9" hidden="1">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>45981</v>
       </c>
@@ -6807,7 +6868,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="217" spans="1:9" hidden="1">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>45981</v>
       </c>
@@ -6830,7 +6891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>45982</v>
       </c>
@@ -6850,7 +6911,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="219" spans="1:9" hidden="1">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>45982</v>
       </c>
@@ -6873,7 +6934,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>45982</v>
       </c>
@@ -6896,7 +6957,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>45982</v>
       </c>
@@ -6919,7 +6980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>45982</v>
       </c>
@@ -6942,7 +7003,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>45982</v>
       </c>
@@ -6965,7 +7026,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>45982</v>
       </c>
@@ -6988,7 +7049,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>45983</v>
       </c>
@@ -7011,7 +7072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>45983</v>
       </c>
@@ -7034,7 +7095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>45984</v>
       </c>
@@ -7057,7 +7118,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>45984</v>
       </c>
@@ -7080,7 +7141,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>45984</v>
       </c>
@@ -7103,7 +7164,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>45985</v>
       </c>
@@ -7123,7 +7184,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>45985</v>
       </c>
@@ -7146,7 +7207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>45985</v>
       </c>
@@ -7169,7 +7230,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>45985</v>
       </c>
@@ -7192,7 +7253,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>45985</v>
       </c>
@@ -7215,7 +7276,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>45985</v>
       </c>
@@ -7238,7 +7299,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>45985</v>
       </c>
@@ -7261,7 +7322,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>45985</v>
       </c>
@@ -7284,7 +7345,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>45985</v>
       </c>
@@ -7307,7 +7368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>45985</v>
       </c>
@@ -7330,7 +7391,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>45985</v>
       </c>
@@ -7350,7 +7411,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>45985</v>
       </c>
@@ -7373,7 +7434,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>45985</v>
       </c>
@@ -7396,7 +7457,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>45985</v>
       </c>
@@ -7419,7 +7480,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>45985</v>
       </c>
@@ -7442,7 +7503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>45985</v>
       </c>
@@ -7465,7 +7526,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>45985</v>
       </c>
@@ -7488,7 +7549,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>45985</v>
       </c>
@@ -7511,7 +7572,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>45985</v>
       </c>
@@ -7531,7 +7592,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>45985</v>
       </c>
@@ -7554,7 +7615,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>45985</v>
       </c>
@@ -7574,7 +7635,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>45986</v>
       </c>
@@ -7597,7 +7658,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>45986</v>
       </c>
@@ -7620,7 +7681,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>45986</v>
       </c>
@@ -7643,7 +7704,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>45986</v>
       </c>
@@ -7666,7 +7727,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>45986</v>
       </c>
@@ -7689,7 +7750,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>45986</v>
       </c>
@@ -7712,7 +7773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:9" hidden="1">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>45986</v>
       </c>
@@ -7732,7 +7793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="258" spans="1:9" hidden="1">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>45986</v>
       </c>
@@ -7755,7 +7816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="259" spans="1:9" hidden="1">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>45986</v>
       </c>
@@ -7778,7 +7839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="260" spans="1:9" hidden="1">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>45986</v>
       </c>
@@ -7801,7 +7862,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="261" spans="1:9" hidden="1">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>45986</v>
       </c>
@@ -7824,7 +7885,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="262" spans="1:9" hidden="1">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>45986</v>
       </c>
@@ -7847,7 +7908,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="263" spans="1:9" hidden="1">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>45987</v>
       </c>
@@ -7867,7 +7928,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="264" spans="1:9" hidden="1">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>45987</v>
       </c>
@@ -7890,7 +7951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="265" spans="1:9" hidden="1">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>45987</v>
       </c>
@@ -7913,7 +7974,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="266" spans="1:9" hidden="1">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>45987</v>
       </c>
@@ -7936,7 +7997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="267" spans="1:9" hidden="1">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>45987</v>
       </c>
@@ -7957,7 +8018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="268" spans="1:9" hidden="1">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>45987</v>
       </c>
@@ -7980,7 +8041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="269" spans="1:9" hidden="1">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>45987</v>
       </c>
@@ -8003,7 +8064,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="270" spans="1:9" hidden="1">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>45987</v>
       </c>
@@ -8026,7 +8087,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="271" spans="1:9" hidden="1">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>45987</v>
       </c>
@@ -8049,7 +8110,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="272" spans="1:9" hidden="1">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>45987</v>
       </c>
@@ -8072,7 +8133,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="273" spans="1:9" hidden="1">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>45987</v>
       </c>
@@ -8092,7 +8153,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="274" spans="1:9" hidden="1">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>45987</v>
       </c>
@@ -8112,7 +8173,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="275" spans="1:9" hidden="1">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>45987</v>
       </c>
@@ -8135,7 +8196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="276" spans="1:9" hidden="1">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>45987</v>
       </c>
@@ -8155,7 +8216,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="277" spans="1:9" hidden="1">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>45987</v>
       </c>
@@ -8178,7 +8239,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="278" spans="1:9" hidden="1">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>45988</v>
       </c>
@@ -8201,7 +8262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="279" spans="1:9" hidden="1">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>45988</v>
       </c>
@@ -8224,7 +8285,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="280" spans="1:9" hidden="1">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>45988</v>
       </c>
@@ -8247,7 +8308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="281" spans="1:9" hidden="1">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>45988</v>
       </c>
@@ -8270,7 +8331,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="282" spans="1:9" hidden="1">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>45988</v>
       </c>
@@ -8293,7 +8354,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="283" spans="1:9" hidden="1">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>45988</v>
       </c>
@@ -8313,7 +8374,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="284" spans="1:9" hidden="1">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>45988</v>
       </c>
@@ -8336,7 +8397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="285" spans="1:9" hidden="1">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>45988</v>
       </c>
@@ -8359,7 +8420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="286" spans="1:9" hidden="1">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>45988</v>
       </c>
@@ -8379,7 +8440,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="287" spans="1:9" hidden="1">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>45988</v>
       </c>
@@ -8402,7 +8463,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="288" spans="1:9" hidden="1">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>45988</v>
       </c>
@@ -8425,7 +8486,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="289" spans="1:9" hidden="1">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>45988</v>
       </c>
@@ -8448,7 +8509,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="290" spans="1:9" hidden="1">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>45988</v>
       </c>
@@ -8471,7 +8532,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="291" spans="1:9" hidden="1">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>45988</v>
       </c>
@@ -8491,7 +8552,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="292" spans="1:9" hidden="1">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>45988</v>
       </c>
@@ -8514,7 +8575,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="293" spans="1:9" hidden="1">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>45988</v>
       </c>
@@ -8537,7 +8598,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="294" spans="1:9" hidden="1">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>45989</v>
       </c>
@@ -8557,7 +8618,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="295" spans="1:9" hidden="1">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>45989</v>
       </c>
@@ -8580,7 +8641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="296" spans="1:9" hidden="1">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>45989</v>
       </c>
@@ -8603,7 +8664,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:9" hidden="1">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>45989</v>
       </c>
@@ -8626,7 +8687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:9" hidden="1">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>45989</v>
       </c>
@@ -8649,7 +8710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:9" hidden="1">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>45989</v>
       </c>
@@ -8672,7 +8733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="300" spans="1:9" hidden="1">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>45989</v>
       </c>
@@ -8695,7 +8756,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="301" spans="1:9" hidden="1">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>45989</v>
       </c>
@@ -8718,7 +8779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="302" spans="1:9" hidden="1">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>45989</v>
       </c>
@@ -8741,7 +8802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="1:9" hidden="1">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>45989</v>
       </c>
@@ -8764,7 +8825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="304" spans="1:9" hidden="1">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>45989</v>
       </c>
@@ -8787,7 +8848,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="305" spans="1:9" hidden="1">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>45989</v>
       </c>
@@ -8810,7 +8871,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="306" spans="1:9" hidden="1">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>45989</v>
       </c>
@@ -8830,7 +8891,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="307" spans="1:9" hidden="1">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>45989</v>
       </c>
@@ -8853,7 +8914,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="308" spans="1:9" hidden="1">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>45989</v>
       </c>
@@ -8876,7 +8937,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="309" spans="1:9" hidden="1">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>45989</v>
       </c>
@@ -8899,7 +8960,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="310" spans="1:9" hidden="1">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>45989</v>
       </c>
@@ -8922,7 +8983,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="311" spans="1:9" hidden="1">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>45990</v>
       </c>
@@ -8945,7 +9006,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="312" spans="1:9" hidden="1">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>45990</v>
       </c>
@@ -8968,7 +9029,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="313" spans="1:9" hidden="1">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>45990</v>
       </c>
@@ -8991,7 +9052,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="314" spans="1:9" hidden="1">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>45990</v>
       </c>
@@ -9014,7 +9075,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="315" spans="1:9" hidden="1">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>45990</v>
       </c>
@@ -9037,7 +9098,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="316" spans="1:9" hidden="1">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>45991</v>
       </c>
@@ -9057,7 +9118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="317" spans="1:9" hidden="1">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>45991</v>
       </c>
@@ -9080,7 +9141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="318" spans="1:9" hidden="1">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>45991</v>
       </c>
@@ -9103,7 +9164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:9" hidden="1">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>45991</v>
       </c>
@@ -9124,45 +9185,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I319" xr:uid="{19B6550E-C6E8-4640-92B4-9AD60B0000E3}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190778206 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190812705 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190859005 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190859506 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190885105 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190885203 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190892600 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/190959705 DD"/>
-        <filter val="TOPAZ FIN JASPER      PRU00010/191462710 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/130654303 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/131188407 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/131992707 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/132514207 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/134121904 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/134332909 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/134333009 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/134338410 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/134467209 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/137376006 DD"/>
-        <filter val="TOPAZ FIN ROSINCA     BLA00010/137376104 DD"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560470501 DD"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560470610 DD"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560470708FIR"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560471505 DD"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560471701FIR"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560471810FIR"/>
-        <filter val="TOPAZ RE ROSINCA      ROW20004/560476808FIR"/>
-        <filter val="TOPAZ RE SIBERITE     SIB00001/480016104 DD"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Mortgage"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I319" xr:uid="{19B6550E-C6E8-4640-92B4-9AD60B0000E3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>